<commit_message>
Do not resize buttons when the column width is larger than the maximum endpoint with buttons.
</commit_message>
<xml_diff>
--- a/Misc/ButtonSizes.xlsx
+++ b/Misc/ButtonSizes.xlsx
@@ -354,7 +354,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1729,24 +1728,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1754,7 +1753,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1768,191 +1767,207 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <f>(B6-D6)/C6</f>
         <v>0</v>
       </c>
       <c r="B6">
         <f>D6</f>
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
         <f>B$1+C6*C$1</f>
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <f t="shared" ref="A7:A27" si="0">(B7-D7)/C7</f>
         <v>110</v>
       </c>
       <c r="B7">
         <f>D7+C7*B$2</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D27" si="1">B$1+C7*C$1</f>
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <f>B7</f>
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="B9">
         <f>D9+C9*B$2</f>
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>72.666666666666671</v>
+        <v>72</v>
       </c>
       <c r="B10">
         <f>B9</f>
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="B11">
         <f>D11+C11*B$2</f>
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>82</v>
+        <v>81.5</v>
       </c>
       <c r="B12">
         <f>B11</f>
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="B13">
         <f>D13+C13*B$2</f>
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F18" si="2">(A13-A12)/2+A12</f>
+        <v>95.75</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:G18" si="3">(B13-B12)/2+B12</f>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>87.6</v>
+        <v>87.2</v>
       </c>
       <c r="B14">
         <f>B13</f>
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C14">
         <v>5</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="B15">
         <f>D15+C15*B$2</f>
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C15">
         <v>5</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>98.6</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>91.333333333333329</v>
+        <v>91</v>
       </c>
       <c r="B16">
         <f>B15</f>
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C16">
         <v>6</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1962,31 +1977,39 @@
       </c>
       <c r="B17">
         <f>D17+C17*B$2</f>
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>100.5</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>707</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>93.714285714285708</v>
       </c>
       <c r="B18">
         <f>B17</f>
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -1996,39 +2019,39 @@
       </c>
       <c r="B19">
         <f>D19+C19*B$2</f>
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="C19">
         <v>7</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F19">
         <f>(A19-A18)/2+A18</f>
-        <v>102</v>
+        <v>101.85714285714286</v>
       </c>
       <c r="G19">
         <f>(B19-B18)/2+B18</f>
-        <v>817</v>
+        <v>821</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>95.75</v>
       </c>
       <c r="B20">
         <f>B19</f>
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="C20">
         <v>8</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -2038,31 +2061,31 @@
       </c>
       <c r="B21">
         <f>D21+C21*B$2</f>
-        <v>985</v>
+        <v>992</v>
       </c>
       <c r="C21">
         <v>8</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>97.555555555555557</v>
+        <v>97.333333333333329</v>
       </c>
       <c r="B22">
         <f>B21</f>
-        <v>985</v>
+        <v>992</v>
       </c>
       <c r="C22">
         <v>9</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -2072,31 +2095,31 @@
       </c>
       <c r="B23">
         <f>D23+C23*B$2</f>
-        <v>1097</v>
+        <v>1106</v>
       </c>
       <c r="C23">
         <v>9</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>98.8</v>
+        <v>98.6</v>
       </c>
       <c r="B24">
         <f>B23</f>
-        <v>1097</v>
+        <v>1106</v>
       </c>
       <c r="C24">
         <v>10</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -2106,31 +2129,31 @@
       </c>
       <c r="B25">
         <f>D25+C25*B$2</f>
-        <v>1209</v>
+        <v>1220</v>
       </c>
       <c r="C25">
         <v>10</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>99.818181818181813</v>
+        <v>99.63636363636364</v>
       </c>
       <c r="B26">
         <f>B25</f>
-        <v>1209</v>
+        <v>1220</v>
       </c>
       <c r="C26">
         <v>11</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
@@ -2140,14 +2163,14 @@
       </c>
       <c r="B27">
         <f>D27+C27*B$2</f>
-        <v>1321</v>
+        <v>1334</v>
       </c>
       <c r="C27">
         <v>11</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>